<commit_message>
Fixed CUDA util and added data precomputation
</commit_message>
<xml_diff>
--- a/Arbeitszeit.xlsx
+++ b/Arbeitszeit.xlsx
@@ -5,13 +5,13 @@
   <workbookPr date1904="1" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Philipp\Studium\Test-Time-Domain-Adaptation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Philipp\Studium\Molecular-Test-Time-Adaptation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BB496F-7C0D-476D-ABCB-D219D83C2746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D8C0FE-204D-40BD-9164-64D5965F1803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="HCoKw4gRij0gV6dkJfNeqDY8SK+w2PMaLYVl2wyqiuSEdbwXoxG0BpbDJ/qeWfNHoSNSKsH2JW6N7mRDHC8t+w==" workbookSaltValue="AxSev/HzJnlnx2x5wdOaWw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="933" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="933" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voreinstellungen" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="145">
   <si>
     <t>Benutzer-Voreinstellungen</t>
   </si>
@@ -585,6 +585,12 @@
   </si>
   <si>
     <t>Literaturrecherche</t>
+  </si>
+  <si>
+    <t>Literaturrecherche und Coding</t>
+  </si>
+  <si>
+    <t>Coding</t>
   </si>
 </sst>
 </file>
@@ -8587,7 +8593,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8632,7 +8638,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8677,7 +8683,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8722,7 +8728,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8767,7 +8773,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8812,7 +8818,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8857,7 +8863,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8902,7 +8908,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8947,7 +8953,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8992,7 +8998,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9037,7 +9043,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9082,7 +9088,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9127,7 +9133,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9172,7 +9178,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9217,7 +9223,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9262,7 +9268,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9307,7 +9313,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9352,7 +9358,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9397,7 +9403,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9442,7 +9448,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9487,7 +9493,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9532,7 +9538,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9577,7 +9583,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9622,7 +9628,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9667,7 +9673,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9712,7 +9718,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9757,7 +9763,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9802,7 +9808,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9847,7 +9853,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9892,7 +9898,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9937,7 +9943,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -9968,7 +9974,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juli!F40</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -10088,7 +10094,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -10598,7 +10604,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10643,7 +10649,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10688,7 +10694,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10733,7 +10739,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10778,7 +10784,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10823,7 +10829,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10868,7 +10874,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10913,7 +10919,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10958,7 +10964,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11003,7 +11009,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11048,7 +11054,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11093,7 +11099,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11138,7 +11144,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11183,7 +11189,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11228,7 +11234,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11273,7 +11279,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11318,7 +11324,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11363,7 +11369,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11408,7 +11414,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11453,7 +11459,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11498,7 +11504,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11543,7 +11549,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11588,7 +11594,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11633,7 +11639,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11678,7 +11684,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11723,7 +11729,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11768,7 +11774,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11813,7 +11819,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11858,7 +11864,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11903,7 +11909,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11979,7 +11985,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">August!F40</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -12099,7 +12105,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -12609,7 +12615,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12654,7 +12660,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12699,7 +12705,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12744,7 +12750,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12789,7 +12795,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12834,7 +12840,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12879,7 +12885,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12924,7 +12930,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12969,7 +12975,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13014,7 +13020,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13059,7 +13065,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13104,7 +13110,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13149,7 +13155,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13194,7 +13200,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13239,7 +13245,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13284,7 +13290,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13329,7 +13335,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13374,7 +13380,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13419,7 +13425,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13464,7 +13470,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13509,7 +13515,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13554,7 +13560,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13599,7 +13605,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13644,7 +13650,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13689,7 +13695,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13734,7 +13740,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13779,7 +13785,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13824,7 +13830,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13869,7 +13875,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13914,7 +13920,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13959,7 +13965,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -13990,7 +13996,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">September!F40</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -14110,7 +14116,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -14620,7 +14626,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14665,7 +14671,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14710,7 +14716,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14755,7 +14761,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14800,7 +14806,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14845,7 +14851,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14890,7 +14896,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14935,7 +14941,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14980,7 +14986,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15025,7 +15031,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15070,7 +15076,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15115,7 +15121,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15160,7 +15166,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15205,7 +15211,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15250,7 +15256,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15295,7 +15301,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15340,7 +15346,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15385,7 +15391,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15430,7 +15436,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15475,7 +15481,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15520,7 +15526,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15565,7 +15571,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15610,7 +15616,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15655,7 +15661,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15700,7 +15706,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15745,7 +15751,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15790,7 +15796,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15835,7 +15841,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15880,7 +15886,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15925,7 +15931,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16001,7 +16007,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Oktober!F40</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -16121,7 +16127,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -16631,7 +16637,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16676,7 +16682,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16721,7 +16727,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16766,7 +16772,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16811,7 +16817,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16856,7 +16862,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16901,7 +16907,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16946,7 +16952,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16991,7 +16997,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17036,7 +17042,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17081,7 +17087,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17126,7 +17132,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17171,7 +17177,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17216,7 +17222,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17261,7 +17267,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17306,7 +17312,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17351,7 +17357,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17396,7 +17402,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17441,7 +17447,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17486,7 +17492,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17531,7 +17537,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17576,7 +17582,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17621,7 +17627,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17666,7 +17672,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17711,7 +17717,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17756,7 +17762,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17801,7 +17807,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17846,7 +17852,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17891,7 +17897,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17936,7 +17942,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17981,7 +17987,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -18012,7 +18018,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">November!F40</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -18132,7 +18138,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -22204,9 +22210,9 @@
         <f>März!A27</f>
         <v>44278</v>
       </c>
-      <c r="I27" s="134" t="str">
+      <c r="I27" s="134">
         <f>IF(März!K27&gt;0,März!K27,"")</f>
-        <v/>
+        <v>0.10416666666666674</v>
       </c>
       <c r="J27" s="125" t="str">
         <f>IF(OR(März!C27="",März!J27&lt;&gt;""),UPPER(März!J27),"F")</f>
@@ -22964,9 +22970,9 @@
         <f>März!A32</f>
         <v>44283</v>
       </c>
-      <c r="I32" s="134" t="str">
+      <c r="I32" s="134">
         <f>IF(März!K32&gt;0,März!K32,"")</f>
-        <v/>
+        <v>9.375E-2</v>
       </c>
       <c r="J32" s="125" t="str">
         <f>IF(OR(März!C32="",März!J32&lt;&gt;""),UPPER(März!J32),"F")</f>
@@ -23487,7 +23493,7 @@
       <c r="G36" s="264"/>
       <c r="H36" s="414">
         <f>März!F38</f>
-        <v>0.20833333333333337</v>
+        <v>0.40625000000000011</v>
       </c>
       <c r="I36" s="414"/>
       <c r="J36" s="265"/>
@@ -23547,7 +23553,7 @@
       <c r="AK36" s="264"/>
       <c r="AL36" s="266">
         <f t="shared" si="0"/>
-        <v>0.20833333333333337</v>
+        <v>0.40625000000000011</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="1" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -23568,7 +23574,7 @@
       <c r="G37" s="82"/>
       <c r="H37" s="409">
         <f ca="1">ROUND(H36-H35,10)</f>
-        <v>-0.41666666670000002</v>
+        <v>-0.21875</v>
       </c>
       <c r="I37" s="409"/>
       <c r="J37" s="83"/>
@@ -23628,7 +23634,7 @@
       <c r="AK37" s="82"/>
       <c r="AL37" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7916666667000001</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="38" spans="1:38" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
@@ -23649,7 +23655,7 @@
       <c r="G38" s="410"/>
       <c r="H38" s="410">
         <f>März!J40</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I38" s="410"/>
       <c r="J38" s="410"/>
@@ -23709,7 +23715,7 @@
       <c r="AK38" s="410"/>
       <c r="AL38" s="343">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
@@ -26064,7 +26070,7 @@
       <c r="D2" s="92"/>
       <c r="E2" s="93">
         <f>Jahresübersicht!AL38</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -30766,10 +30772,10 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="O28" sqref="O28"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -31950,8 +31956,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D27" s="325"/>
-      <c r="E27" s="325"/>
+      <c r="D27" s="325">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E27" s="325">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="F27" s="325"/>
       <c r="G27" s="325"/>
       <c r="H27" s="326"/>
@@ -31962,7 +31972,7 @@
       <c r="J27" s="163"/>
       <c r="K27" s="319">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.10416666666666674</v>
       </c>
       <c r="L27" s="320">
         <f t="shared" ca="1" si="3"/>
@@ -31970,16 +31980,18 @@
       </c>
       <c r="M27" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>-2.0833333333330002E-2</v>
       </c>
       <c r="N27" s="360">
         <f t="shared" ca="1" si="5"/>
         <v>0.125</v>
       </c>
-      <c r="O27" s="165"/>
+      <c r="O27" s="165" t="s">
+        <v>143</v>
+      </c>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.29166666666666002</v>
+        <v>-0.18749999999999001</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32024,7 +32036,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.29166666666666002</v>
+        <v>-0.18749999999999001</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32069,7 +32081,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.29166666666666002</v>
+        <v>-0.18749999999999001</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32114,7 +32126,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.29166666666666002</v>
+        <v>-0.18749999999999001</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32159,7 +32171,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.29166666666666002</v>
+        <v>-0.18749999999999001</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32175,8 +32187,12 @@
         <f>IF(ISERROR(VLOOKUP(A32,Feiertage,2,FALSE)),"",(VLOOKUP(A32,Feiertage,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="D32" s="325"/>
-      <c r="E32" s="325"/>
+      <c r="D32" s="325">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E32" s="325">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="F32" s="325"/>
       <c r="G32" s="325"/>
       <c r="H32" s="326"/>
@@ -32187,7 +32203,7 @@
       <c r="J32" s="163"/>
       <c r="K32" s="319">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.375E-2</v>
       </c>
       <c r="L32" s="320">
         <f t="shared" ca="1" si="3"/>
@@ -32195,16 +32211,18 @@
       </c>
       <c r="M32" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>9.375E-2</v>
       </c>
       <c r="N32" s="360">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
-      <c r="O32" s="165"/>
+      <c r="O32" s="165" t="s">
+        <v>144</v>
+      </c>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.29166666666666002</v>
+        <v>-9.3749999999989994E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32249,7 +32267,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.29166666666666002</v>
+        <v>-9.3749999999989994E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32294,7 +32312,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-0.41666666666666002</v>
+        <v>-0.21874999999999001</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -32389,7 +32407,7 @@
       </c>
       <c r="F38" s="171">
         <f>SUM(K4:K34)</f>
-        <v>0.20833333333333337</v>
+        <v>0.40625000000000011</v>
       </c>
       <c r="G38" s="53"/>
       <c r="I38" s="68"/>
@@ -32445,13 +32463,13 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.41666666666667002</v>
+        <v>-0.21875</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
       <c r="J40" s="210">
         <f>COUNTIF(K4:K34,"&gt;0")-IF(Voreinstellungen!C28="XTRA",COUNTIF(J4:J34,Voreinstellungen!B28),0)-IF(Voreinstellungen!C29="XTRA",COUNTIF(J4:J34,Voreinstellungen!B29),0)-IF(Voreinstellungen!C30="XTRA",COUNTIF(J4:J34,Voreinstellungen!B30),0)-IF(Voreinstellungen!C31="XTRA",COUNTIF(J4:J34,Voreinstellungen!B31),0)-IF(Voreinstellungen!C32="XTRA",COUNTIF(J4:J34,Voreinstellungen!B32),0)-IF(Voreinstellungen!C33="XTRA",COUNTIF(J4:J34,Voreinstellungen!B33),0)-COUNTIF(J4:J34,"H")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K40" s="380" t="s">
         <v>91</v>
@@ -32955,7 +32973,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.41666666666667002</v>
+        <v>-0.21875</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33000,7 +33018,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.41666666666667002</v>
+        <v>-0.21875</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33045,7 +33063,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.41666666666667002</v>
+        <v>-0.21875</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33090,7 +33108,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.41666666666667002</v>
+        <v>-0.21875</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33135,7 +33153,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.41666666666667002</v>
+        <v>-0.21875</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33180,7 +33198,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.41666666666667002</v>
+        <v>-0.21875</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33225,7 +33243,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.54166666666666996</v>
+        <v>-0.34375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33270,7 +33288,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.54166666666666996</v>
+        <v>-0.34375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33315,7 +33333,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.54166666666666996</v>
+        <v>-0.34375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33360,7 +33378,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.54166666666666996</v>
+        <v>-0.34375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33405,7 +33423,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.54166666666666996</v>
+        <v>-0.34375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33450,7 +33468,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.54166666666666996</v>
+        <v>-0.34375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33495,7 +33513,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.54166666666666996</v>
+        <v>-0.34375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33540,7 +33558,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33585,7 +33603,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33630,7 +33648,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33675,7 +33693,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33720,7 +33738,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33765,7 +33783,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33810,7 +33828,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33855,7 +33873,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33900,7 +33918,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33945,7 +33963,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33990,7 +34008,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34035,7 +34053,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34080,7 +34098,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34125,7 +34143,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.66666666666666996</v>
+        <v>-0.46875</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34170,7 +34188,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.79166666666666996</v>
+        <v>-0.59375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34215,7 +34233,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.79166666666666996</v>
+        <v>-0.59375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34260,7 +34278,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.79166666666666996</v>
+        <v>-0.59375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34336,7 +34354,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">März!F40</f>
-        <v>-0.41666666666667002</v>
+        <v>-0.21875</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -34456,7 +34474,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.79166666666666996</v>
+        <v>-0.59375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -34966,7 +34984,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.79166666666666996</v>
+        <v>-0.59375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35011,7 +35029,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.79166666666666996</v>
+        <v>-0.59375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35056,7 +35074,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.79166666666666996</v>
+        <v>-0.59375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35101,7 +35119,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.79166666666666996</v>
+        <v>-0.59375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35146,7 +35164,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.91666666666666996</v>
+        <v>-0.71875</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35191,7 +35209,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.91666666666666996</v>
+        <v>-0.71875</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35236,7 +35254,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.91666666666666996</v>
+        <v>-0.71875</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35281,7 +35299,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.91666666666666996</v>
+        <v>-0.71875</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35326,7 +35344,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.91666666666666996</v>
+        <v>-0.71875</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35371,7 +35389,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.91666666666666996</v>
+        <v>-0.71875</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35416,7 +35434,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.91666666666666996</v>
+        <v>-0.71875</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35461,7 +35479,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.0416666666666701</v>
+        <v>-0.84375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35506,7 +35524,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.0416666666666701</v>
+        <v>-0.84375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35551,7 +35569,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.0416666666666701</v>
+        <v>-0.84375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35596,7 +35614,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.0416666666666701</v>
+        <v>-0.84375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35641,7 +35659,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.0416666666666701</v>
+        <v>-0.84375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35686,7 +35704,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.0416666666666701</v>
+        <v>-0.84375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35731,7 +35749,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.0416666666666701</v>
+        <v>-0.84375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35776,7 +35794,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1666666666666701</v>
+        <v>-0.96875</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35821,7 +35839,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1666666666666701</v>
+        <v>-0.96875</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35866,7 +35884,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1666666666666701</v>
+        <v>-0.96875</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35911,7 +35929,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1666666666666701</v>
+        <v>-0.96875</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35956,7 +35974,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1666666666666701</v>
+        <v>-0.96875</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36001,7 +36019,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1666666666666701</v>
+        <v>-0.96875</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36046,7 +36064,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1666666666666701</v>
+        <v>-0.96875</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36091,7 +36109,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.2916666666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36136,7 +36154,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.2916666666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36181,7 +36199,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.2916666666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36226,7 +36244,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.2916666666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36271,7 +36289,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.2916666666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36316,7 +36334,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.2916666666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -36347,7 +36365,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">April!F40</f>
-        <v>-0.79166666666666996</v>
+        <v>-0.59375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -36467,7 +36485,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.2916666666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -36977,7 +36995,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.2916666666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37022,7 +37040,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37067,7 +37085,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37112,7 +37130,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37157,7 +37175,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37202,7 +37220,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37247,7 +37265,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37292,7 +37310,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37337,7 +37355,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37382,7 +37400,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37427,7 +37445,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37472,7 +37490,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37517,7 +37535,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37562,7 +37580,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37607,7 +37625,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4166666666666701</v>
+        <v>-1.21875</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37652,7 +37670,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.5416666666666701</v>
+        <v>-1.34375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37697,7 +37715,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.5416666666666701</v>
+        <v>-1.34375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37742,7 +37760,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.5416666666666701</v>
+        <v>-1.34375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37787,7 +37805,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.5416666666666701</v>
+        <v>-1.34375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37832,7 +37850,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.5416666666666701</v>
+        <v>-1.34375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37877,7 +37895,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.5416666666666701</v>
+        <v>-1.34375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37922,7 +37940,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.5416666666666701</v>
+        <v>-1.34375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37967,7 +37985,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.6666666666666701</v>
+        <v>-1.46875</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38012,7 +38030,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.6666666666666701</v>
+        <v>-1.46875</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38057,7 +38075,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.6666666666666701</v>
+        <v>-1.46875</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38102,7 +38120,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.6666666666666701</v>
+        <v>-1.46875</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38147,7 +38165,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.6666666666666701</v>
+        <v>-1.46875</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38192,7 +38210,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.6666666666666701</v>
+        <v>-1.46875</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38237,7 +38255,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.6666666666666701</v>
+        <v>-1.46875</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38282,7 +38300,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38358,7 +38376,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Mai!F40</f>
-        <v>-1.2916666666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -38478,7 +38496,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -38828,7 +38846,7 @@
   </sheetPr>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
@@ -38988,7 +39006,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39033,7 +39051,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39078,7 +39096,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39123,7 +39141,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39168,7 +39186,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39213,7 +39231,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39258,7 +39276,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39303,7 +39321,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39348,7 +39366,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39393,7 +39411,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39438,7 +39456,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39483,7 +39501,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39528,7 +39546,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39573,7 +39591,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39618,7 +39636,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39663,7 +39681,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39708,7 +39726,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39753,7 +39771,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39798,7 +39816,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39843,7 +39861,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39888,7 +39906,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39933,7 +39951,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39978,7 +39996,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40023,7 +40041,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40068,7 +40086,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40113,7 +40131,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40158,7 +40176,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40203,7 +40221,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40248,7 +40266,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40293,7 +40311,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40338,7 +40356,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -40369,7 +40387,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juni!F40</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -40489,7 +40507,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.7916666666666701</v>
+        <v>-1.59375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>

</xml_diff>

<commit_message>
Added embedding analysis and model loading
</commit_message>
<xml_diff>
--- a/Arbeitszeit.xlsx
+++ b/Arbeitszeit.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Philipp\Studium\Molecular-Test-Time-Adaptation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910145E1-625A-4398-A99E-AC3D2C3802E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741F7480-CAA7-4847-8302-A4CB63847526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="HCoKw4gRij0gV6dkJfNeqDY8SK+w2PMaLYVl2wyqiuSEdbwXoxG0BpbDJ/qeWfNHoSNSKsH2JW6N7mRDHC8t+w==" workbookSaltValue="AxSev/HzJnlnx2x5wdOaWw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" tabRatio="933" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="933" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voreinstellungen" sheetId="1" r:id="rId1"/>
@@ -7880,7 +7880,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="11.4" x14ac:dyDescent="0.25"/>
@@ -8079,14 +8079,14 @@
         <v>19</v>
       </c>
       <c r="B13" s="143">
-        <v>44255</v>
+        <v>44376</v>
       </c>
       <c r="C13" s="15">
         <f>IF(B13="","",SUM(D13:J13))</f>
-        <v>0.125</v>
+        <v>3.125</v>
       </c>
       <c r="D13" s="155">
-        <v>0.125</v>
+        <v>3.125</v>
       </c>
       <c r="E13" s="156">
         <v>0</v>
@@ -8368,7 +8368,7 @@
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="273">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -8387,7 +8387,7 @@
       <c r="B38" s="23"/>
       <c r="C38" s="275">
         <f>SUM(C36:C37)-Jahresübersicht!AL43</f>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
@@ -8593,7 +8593,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8638,7 +8638,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8683,7 +8683,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8728,7 +8728,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8773,7 +8773,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8818,7 +8818,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8863,7 +8863,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8908,7 +8908,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8953,7 +8953,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8998,7 +8998,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9043,7 +9043,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9088,7 +9088,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9133,7 +9133,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9178,7 +9178,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9223,7 +9223,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9268,7 +9268,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9313,7 +9313,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9358,7 +9358,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9403,7 +9403,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9448,7 +9448,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9493,7 +9493,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9538,7 +9538,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9583,7 +9583,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9628,7 +9628,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9673,7 +9673,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9718,7 +9718,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9763,7 +9763,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9808,7 +9808,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9853,7 +9853,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9898,7 +9898,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9943,7 +9943,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -9974,7 +9974,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juli!F40</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -10016,7 +10016,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -10094,7 +10094,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -10604,7 +10604,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10649,7 +10649,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10694,7 +10694,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10739,7 +10739,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10784,7 +10784,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10829,7 +10829,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10874,7 +10874,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10919,7 +10919,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10964,7 +10964,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11009,7 +11009,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11054,7 +11054,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11099,7 +11099,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11144,7 +11144,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11189,7 +11189,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11234,7 +11234,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11279,7 +11279,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11324,7 +11324,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11369,7 +11369,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11414,7 +11414,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11459,7 +11459,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11504,7 +11504,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11549,7 +11549,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11594,7 +11594,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11639,7 +11639,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11684,7 +11684,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11729,7 +11729,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11774,7 +11774,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11819,7 +11819,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11864,7 +11864,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11909,7 +11909,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11985,7 +11985,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">August!F40</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -12027,7 +12027,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -12105,7 +12105,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -12615,7 +12615,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12660,7 +12660,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12705,7 +12705,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12750,7 +12750,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12795,7 +12795,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12840,7 +12840,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12885,7 +12885,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12930,7 +12930,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12975,7 +12975,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13020,7 +13020,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13065,7 +13065,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13110,7 +13110,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13155,7 +13155,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13200,7 +13200,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13245,7 +13245,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13290,7 +13290,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13335,7 +13335,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13380,7 +13380,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13425,7 +13425,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13470,7 +13470,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13515,7 +13515,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13560,7 +13560,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13605,7 +13605,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13650,7 +13650,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13695,7 +13695,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13740,7 +13740,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13785,7 +13785,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13830,7 +13830,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13875,7 +13875,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13920,7 +13920,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13965,7 +13965,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -13996,7 +13996,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">September!F40</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -14038,7 +14038,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -14116,7 +14116,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -14626,7 +14626,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14671,7 +14671,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14716,7 +14716,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14761,7 +14761,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14806,7 +14806,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14851,7 +14851,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14896,7 +14896,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14941,7 +14941,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14986,7 +14986,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15031,7 +15031,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15076,7 +15076,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15121,7 +15121,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15166,7 +15166,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15211,7 +15211,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15256,7 +15256,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15301,7 +15301,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15346,7 +15346,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15391,7 +15391,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15436,7 +15436,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15481,7 +15481,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15526,7 +15526,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15571,7 +15571,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15616,7 +15616,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15661,7 +15661,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15706,7 +15706,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15751,7 +15751,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15796,7 +15796,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15841,7 +15841,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15886,7 +15886,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15931,7 +15931,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16007,7 +16007,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Oktober!F40</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -16049,7 +16049,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -16127,7 +16127,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -16637,7 +16637,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16682,7 +16682,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16727,7 +16727,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16772,7 +16772,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16817,7 +16817,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16862,7 +16862,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16907,7 +16907,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16952,7 +16952,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16997,7 +16997,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17042,7 +17042,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17087,7 +17087,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17132,7 +17132,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17177,7 +17177,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17222,7 +17222,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17267,7 +17267,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17312,7 +17312,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17357,7 +17357,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17402,7 +17402,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17447,7 +17447,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17492,7 +17492,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17537,7 +17537,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17582,7 +17582,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17627,7 +17627,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17672,7 +17672,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17717,7 +17717,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17762,7 +17762,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17807,7 +17807,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17852,7 +17852,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17897,7 +17897,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17942,7 +17942,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17987,7 +17987,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -18018,7 +18018,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">November!F40</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -18060,7 +18060,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -18138,7 +18138,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -18728,7 +18728,7 @@
       </c>
       <c r="L4" s="133">
         <f>IF(April!K4&gt;0,April!K4,"")</f>
-        <v>4.1666666666666685E-2</v>
+        <v>0.19791666666666663</v>
       </c>
       <c r="M4" s="120" t="str">
         <f>IF(OR(April!C4="",April!J4&lt;&gt;""),UPPER(April!J4),"F")</f>
@@ -23412,25 +23412,25 @@
       <c r="G35" s="260"/>
       <c r="H35" s="412">
         <f ca="1">März!F37</f>
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="I35" s="412"/>
       <c r="J35" s="261"/>
       <c r="K35" s="411">
         <f ca="1">April!F37</f>
-        <v>0.375</v>
+        <v>0</v>
       </c>
       <c r="L35" s="411"/>
       <c r="M35" s="260"/>
       <c r="N35" s="412">
         <f ca="1">Mai!F37</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O35" s="412"/>
       <c r="P35" s="261"/>
       <c r="Q35" s="411">
         <f ca="1">Juni!F37</f>
-        <v>0.5</v>
+        <v>3.125</v>
       </c>
       <c r="R35" s="411"/>
       <c r="S35" s="260"/>
@@ -23472,7 +23472,7 @@
       <c r="AK35" s="260"/>
       <c r="AL35" s="262">
         <f t="shared" ref="AL35:AL50" ca="1" si="0">SUM(B35:AK35)</f>
-        <v>2</v>
+        <v>3.125</v>
       </c>
     </row>
     <row r="36" spans="1:38" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -23499,7 +23499,7 @@
       <c r="J36" s="265"/>
       <c r="K36" s="413">
         <f>April!F38</f>
-        <v>4.1666666666666685E-2</v>
+        <v>0.19791666666666663</v>
       </c>
       <c r="L36" s="413"/>
       <c r="M36" s="264"/>
@@ -23553,7 +23553,7 @@
       <c r="AK36" s="264"/>
       <c r="AL36" s="266">
         <f t="shared" si="0"/>
-        <v>0.84375</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="1" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -23574,25 +23574,25 @@
       <c r="G37" s="82"/>
       <c r="H37" s="409">
         <f ca="1">ROUND(H36-H35,10)</f>
-        <v>0.17708333330000001</v>
+        <v>0.80208333330000003</v>
       </c>
       <c r="I37" s="409"/>
       <c r="J37" s="83"/>
       <c r="K37" s="408">
         <f ca="1">ROUND(K36-K35,10)</f>
-        <v>-0.33333333329999998</v>
+        <v>0.19791666669999999</v>
       </c>
       <c r="L37" s="408"/>
       <c r="M37" s="82"/>
       <c r="N37" s="409">
         <f ca="1">ROUND(N36-N35,10)</f>
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="O37" s="409"/>
       <c r="P37" s="83"/>
       <c r="Q37" s="408">
         <f ca="1">ROUND(Q36-Q35,10)</f>
-        <v>-0.5</v>
+        <v>-3.125</v>
       </c>
       <c r="R37" s="408"/>
       <c r="S37" s="82"/>
@@ -23634,7 +23634,7 @@
       <c r="AK37" s="82"/>
       <c r="AL37" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="38" spans="1:38" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
@@ -28333,7 +28333,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -30344,7 +30344,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -30773,7 +30773,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
@@ -31009,20 +31009,20 @@
       </c>
       <c r="L6" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M6" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N6" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31067,7 +31067,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31112,7 +31112,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31157,7 +31157,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31202,7 +31202,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31247,7 +31247,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31292,7 +31292,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31324,20 +31324,20 @@
       </c>
       <c r="L13" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M13" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N13" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31382,7 +31382,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31427,7 +31427,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31472,7 +31472,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31517,7 +31517,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31562,7 +31562,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31607,7 +31607,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31643,22 +31643,22 @@
       </c>
       <c r="L20" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M20" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.0833333333330002E-2</v>
+        <v>0.10416666666667</v>
       </c>
       <c r="N20" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O20" s="165" t="s">
         <v>142</v>
       </c>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.27083333333332998</v>
+        <v>0.10416666666667</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31709,7 +31709,7 @@
       </c>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.20833333333333001</v>
+        <v>0.16666666666666999</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31754,7 +31754,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.20833333333333001</v>
+        <v>0.16666666666666999</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31799,7 +31799,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.20833333333333001</v>
+        <v>0.16666666666666999</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31844,7 +31844,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.20833333333333001</v>
+        <v>0.16666666666666999</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31889,7 +31889,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.20833333333333001</v>
+        <v>0.16666666666666999</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31940,7 +31940,7 @@
       </c>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.16666666666666</v>
+        <v>0.20833333333334</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -31976,22 +31976,22 @@
       </c>
       <c r="L27" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M27" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.0833333333330002E-2</v>
+        <v>0.10416666666667</v>
       </c>
       <c r="N27" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O27" s="165" t="s">
         <v>143</v>
       </c>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.18749999999999001</v>
+        <v>0.31250000000000999</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32036,7 +32036,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.18749999999999001</v>
+        <v>0.31250000000000999</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32081,7 +32081,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.18749999999999001</v>
+        <v>0.31250000000000999</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32126,7 +32126,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.18749999999999001</v>
+        <v>0.31250000000000999</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32171,7 +32171,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.18749999999999001</v>
+        <v>0.31250000000000999</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32222,7 +32222,7 @@
       </c>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-9.3749999999989994E-2</v>
+        <v>0.40625000000000999</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32273,7 +32273,7 @@
       </c>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>0.12500000000000999</v>
+        <v>0.62500000000000999</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32309,22 +32309,22 @@
       </c>
       <c r="L34" s="322">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M34" s="309">
         <f ca="1">IF(A34="",0,ROUND(K34-L34,14))</f>
-        <v>5.2083333333329998E-2</v>
+        <v>0.17708333333333001</v>
       </c>
       <c r="N34" s="361">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O34" s="310" t="s">
         <v>144</v>
       </c>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>0.17708333333334</v>
+        <v>0.80208333333334003</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -32387,7 +32387,7 @@
       </c>
       <c r="F37" s="170">
         <f ca="1">SUM(L4:L34)</f>
-        <v>0.625</v>
+        <v>0</v>
       </c>
       <c r="G37" s="53"/>
       <c r="I37" s="68"/>
@@ -32397,7 +32397,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -32475,7 +32475,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>0.17708333333333001</v>
+        <v>0.80208333333333004</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -32828,7 +32828,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -32960,7 +32960,7 @@
         <v>0.4375</v>
       </c>
       <c r="E4" s="323">
-        <v>0.47916666666666669</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="F4" s="323"/>
       <c r="G4" s="323"/>
@@ -32972,7 +32972,7 @@
       <c r="J4" s="299"/>
       <c r="K4" s="317">
         <f>IF(A4="",0,IF(IF(D4&lt;E4,E4-D4,IF(E4="",0,E4-D4+1))+IF(F4&lt;G4,G4-F4,IF(G4="",0,G4-F4+1))-H4&gt;0,IF(D4&lt;E4,E4-D4,IF(E4="",0,E4-D4+1))+IF(F4&lt;G4,G4-F4,IF(G4="",0,G4-F4+1))-H4,0))</f>
-        <v>4.1666666666666685E-2</v>
+        <v>0.19791666666666663</v>
       </c>
       <c r="L4" s="318">
         <f t="shared" ref="L4:L34" ca="1" si="3">IF(AND(C4&lt;&gt;"",J4=""),IF(ISERROR(VLOOKUP(B4,Feiertage,2,FALSE)),0,VLOOKUP(B4,Feiertage,3,FALSE)*N4),IF(A4="",0,IF(J4&lt;&gt;"",IF(UPPER(J4)=VLOOKUP(UPPER(J4),Code,1,FALSE),IF(OR(VLOOKUP(J4,Code,2,FALSE)="NONE",VLOOKUP(J4,Code,2,FALSE)="XTRA",VLOOKUP(J4,Code,2,FALSE)="REST"),K4,IF(ISERROR(VLOOKUP(B4,Feiertage,2,FALSE)),VLOOKUP(J4,Code,2,FALSE)*N4,IF(VLOOKUP(B4,Feiertage,3,FALSE)=0.5,IF(OR(UPPER(J4)="G",UPPER(J4)="H"),VLOOKUP(B4,Feiertage,3,FALSE)*VLOOKUP(J4,Code,2,FALSE)*N4,0),VLOOKUP(B4,Feiertage,3,FALSE)*VLOOKUP(J4,Code,2,FALSE)*N4))),N4),N4)))</f>
@@ -32980,7 +32980,7 @@
       </c>
       <c r="M4" s="300">
         <f t="shared" ref="M4:M33" ca="1" si="4">IF(A4="",0,ROUND(K4-L4,14))</f>
-        <v>4.1666666666670002E-2</v>
+        <v>0.19791666666666999</v>
       </c>
       <c r="N4" s="359">
         <f t="shared" ref="N4:N34" ca="1" si="5">IF(A4="",0,INDIRECT(ADDRESS(MATCH(A4,SOLL_AZ_Ab,1)+11,WEEKDAY(A4,2)+3,,,"Voreinstellungen"),TRUE))</f>
@@ -32989,7 +32989,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>0.21875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33034,7 +33034,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>0.21875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33079,7 +33079,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>0.21875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33124,7 +33124,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>0.21875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33169,7 +33169,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>0.21875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33214,7 +33214,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>0.21875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33246,20 +33246,20 @@
       </c>
       <c r="L10" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M10" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N10" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>9.375E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33304,7 +33304,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>9.375E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33349,7 +33349,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>9.375E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33394,7 +33394,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>9.375E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33439,7 +33439,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>9.375E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33484,7 +33484,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>9.375E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33529,7 +33529,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>9.375E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33561,20 +33561,20 @@
       </c>
       <c r="L17" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M17" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N17" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33619,7 +33619,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33664,7 +33664,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33709,7 +33709,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33754,7 +33754,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33799,7 +33799,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33844,7 +33844,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33884,12 +33884,12 @@
       </c>
       <c r="N24" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33934,7 +33934,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33979,7 +33979,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34024,7 +34024,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34069,7 +34069,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34114,7 +34114,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34159,7 +34159,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.125E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34191,20 +34191,20 @@
       </c>
       <c r="L31" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M31" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N31" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.15625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34249,7 +34249,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.15625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34294,7 +34294,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.15625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34370,7 +34370,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">März!F40</f>
-        <v>0.17708333333333001</v>
+        <v>0.80208333333333004</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -34402,7 +34402,7 @@
       </c>
       <c r="F37" s="170">
         <f ca="1">SUM(L4:L34)</f>
-        <v>0.375</v>
+        <v>0</v>
       </c>
       <c r="G37" s="53"/>
       <c r="I37" s="68"/>
@@ -34412,7 +34412,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -34434,7 +34434,7 @@
       </c>
       <c r="F38" s="171">
         <f>SUM(K4:K34)</f>
-        <v>4.1666666666666685E-2</v>
+        <v>0.19791666666666663</v>
       </c>
       <c r="G38" s="53"/>
       <c r="I38" s="68"/>
@@ -34490,7 +34490,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.15625</v>
+        <v>1</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -35000,7 +35000,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.15625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35045,7 +35045,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.15625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35090,7 +35090,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.15625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35135,7 +35135,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.15625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35167,20 +35167,20 @@
       </c>
       <c r="L8" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M8" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N8" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.28125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35225,7 +35225,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.28125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35270,7 +35270,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.28125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35315,7 +35315,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.28125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35360,7 +35360,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.28125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35405,7 +35405,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.28125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35450,7 +35450,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.28125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35482,20 +35482,20 @@
       </c>
       <c r="L15" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M15" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N15" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.40625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35540,7 +35540,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.40625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35585,7 +35585,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.40625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35630,7 +35630,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.40625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35675,7 +35675,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.40625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35720,7 +35720,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.40625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35765,7 +35765,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.40625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35797,20 +35797,20 @@
       </c>
       <c r="L22" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M22" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N22" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.53125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35855,7 +35855,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.53125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35900,7 +35900,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.53125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35945,7 +35945,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.53125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35990,7 +35990,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.53125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36035,7 +36035,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.53125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36080,7 +36080,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.53125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36112,20 +36112,20 @@
       </c>
       <c r="L29" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M29" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N29" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.65625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36170,7 +36170,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.65625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36215,7 +36215,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.65625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36260,7 +36260,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.65625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36305,7 +36305,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.65625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36350,7 +36350,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-0.65625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -36381,7 +36381,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">April!F40</f>
-        <v>-0.15625</v>
+        <v>1</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -36413,7 +36413,7 @@
       </c>
       <c r="F37" s="170">
         <f ca="1">SUM(L4:L34)</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G37" s="53"/>
       <c r="I37" s="68"/>
@@ -36423,7 +36423,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -36501,7 +36501,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.65625</v>
+        <v>1</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -37011,7 +37011,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.65625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37043,20 +37043,20 @@
       </c>
       <c r="L5" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M5" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N5" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37101,7 +37101,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37146,7 +37146,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37191,7 +37191,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37236,7 +37236,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37281,7 +37281,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37326,7 +37326,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37366,12 +37366,12 @@
       </c>
       <c r="N12" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37416,7 +37416,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37461,7 +37461,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37506,7 +37506,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37551,7 +37551,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37596,7 +37596,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37641,7 +37641,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.78125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37673,20 +37673,20 @@
       </c>
       <c r="L19" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M19" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N19" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.90625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37731,7 +37731,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.90625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37776,7 +37776,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.90625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37821,7 +37821,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.90625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37866,7 +37866,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.90625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37911,7 +37911,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.90625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37956,7 +37956,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.90625</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37988,20 +37988,20 @@
       </c>
       <c r="L26" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="M26" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>0</v>
       </c>
       <c r="N26" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.03125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38046,7 +38046,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.03125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38091,7 +38091,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.03125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38136,7 +38136,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.03125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38181,7 +38181,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.03125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38226,7 +38226,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.03125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38271,7 +38271,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.03125</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38303,20 +38303,20 @@
       </c>
       <c r="L33" s="320">
         <f t="shared" ca="1" si="3"/>
-        <v>0.125</v>
+        <v>3.125</v>
       </c>
       <c r="M33" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.125</v>
+        <v>-3.125</v>
       </c>
       <c r="N33" s="360">
         <f t="shared" ca="1" si="5"/>
-        <v>0.125</v>
+        <v>3.125</v>
       </c>
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38392,7 +38392,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Mai!F40</f>
-        <v>-0.65625</v>
+        <v>1</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -38424,7 +38424,7 @@
       </c>
       <c r="F37" s="170">
         <f ca="1">SUM(L4:L34)</f>
-        <v>0.5</v>
+        <v>3.125</v>
       </c>
       <c r="G37" s="53"/>
       <c r="I37" s="68"/>
@@ -38434,7 +38434,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -38512,7 +38512,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -39022,7 +39022,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39067,7 +39067,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39112,7 +39112,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39157,7 +39157,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39202,7 +39202,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39247,7 +39247,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39292,7 +39292,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39337,7 +39337,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39382,7 +39382,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39427,7 +39427,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39472,7 +39472,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39517,7 +39517,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39562,7 +39562,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39607,7 +39607,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39652,7 +39652,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39697,7 +39697,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39742,7 +39742,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39787,7 +39787,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39832,7 +39832,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39877,7 +39877,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39922,7 +39922,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39967,7 +39967,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40012,7 +40012,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40057,7 +40057,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40102,7 +40102,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40147,7 +40147,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40192,7 +40192,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40237,7 +40237,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40282,7 +40282,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40327,7 +40327,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40372,7 +40372,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -40403,7 +40403,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juni!F40</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -40445,7 +40445,7 @@
       </c>
       <c r="K37" s="381" t="str">
         <f>Voreinstellungen!A25&amp;" ("&amp;Voreinstellungen!B25&amp;"/"&amp;Voreinstellungen!B26&amp;") aktuell noch Verfügbar: "&amp;Voreinstellungen!C38&amp;" Tag(e)"</f>
-        <v>Urlaub (U/UH) aktuell noch Verfügbar: 30 Tag(e)</v>
+        <v>Urlaub (U/UH) aktuell noch Verfügbar: 0 Tag(e)</v>
       </c>
       <c r="L37" s="392"/>
       <c r="M37" s="392"/>
@@ -40523,7 +40523,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.15625</v>
+        <v>-2.125</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>

</xml_diff>

<commit_message>
Improvements for batching and GPU util by Esther
</commit_message>
<xml_diff>
--- a/Arbeitszeit.xlsx
+++ b/Arbeitszeit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr date1904="1" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Philipp\Studium\Molecular-Test-Time-Adaptation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741F7480-CAA7-4847-8302-A4CB63847526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22649D9-A970-484A-A33A-D143D1DF2AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="HCoKw4gRij0gV6dkJfNeqDY8SK+w2PMaLYVl2wyqiuSEdbwXoxG0BpbDJ/qeWfNHoSNSKsH2JW6N7mRDHC8t+w==" workbookSaltValue="AxSev/HzJnlnx2x5wdOaWw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="933" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="145">
   <si>
     <t>Benutzer-Voreinstellungen</t>
   </si>
@@ -8593,7 +8593,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8638,7 +8638,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8683,7 +8683,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8728,7 +8728,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8773,7 +8773,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8818,7 +8818,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8863,7 +8863,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8908,7 +8908,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8953,7 +8953,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8998,7 +8998,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9043,7 +9043,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9088,7 +9088,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9133,7 +9133,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9178,7 +9178,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9223,7 +9223,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9268,7 +9268,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9313,7 +9313,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9358,7 +9358,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9403,7 +9403,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9448,7 +9448,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9493,7 +9493,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9538,7 +9538,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9583,7 +9583,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9628,7 +9628,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9673,7 +9673,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9718,7 +9718,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9763,7 +9763,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9808,7 +9808,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9853,7 +9853,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9898,7 +9898,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9943,7 +9943,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -9974,7 +9974,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juli!F40</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -10094,7 +10094,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -10604,7 +10604,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10649,7 +10649,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10694,7 +10694,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10739,7 +10739,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10784,7 +10784,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10829,7 +10829,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10874,7 +10874,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10919,7 +10919,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10964,7 +10964,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11009,7 +11009,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11054,7 +11054,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11099,7 +11099,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11144,7 +11144,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11189,7 +11189,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11234,7 +11234,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11279,7 +11279,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11324,7 +11324,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11369,7 +11369,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11414,7 +11414,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11459,7 +11459,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11504,7 +11504,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11549,7 +11549,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11594,7 +11594,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11639,7 +11639,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11684,7 +11684,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11729,7 +11729,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11774,7 +11774,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11819,7 +11819,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11864,7 +11864,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11909,7 +11909,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11985,7 +11985,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">August!F40</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -12105,7 +12105,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -12615,7 +12615,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12660,7 +12660,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12705,7 +12705,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12750,7 +12750,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12795,7 +12795,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12840,7 +12840,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12885,7 +12885,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12930,7 +12930,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12975,7 +12975,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13020,7 +13020,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13065,7 +13065,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13110,7 +13110,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13155,7 +13155,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13200,7 +13200,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13245,7 +13245,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13290,7 +13290,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13335,7 +13335,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13380,7 +13380,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13425,7 +13425,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13470,7 +13470,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13515,7 +13515,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13560,7 +13560,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13605,7 +13605,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13650,7 +13650,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13695,7 +13695,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13740,7 +13740,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13785,7 +13785,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13830,7 +13830,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13875,7 +13875,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13920,7 +13920,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13965,7 +13965,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -13996,7 +13996,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">September!F40</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -14116,7 +14116,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -14626,7 +14626,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14671,7 +14671,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14716,7 +14716,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14761,7 +14761,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14806,7 +14806,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14851,7 +14851,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14896,7 +14896,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14941,7 +14941,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14986,7 +14986,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15031,7 +15031,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15076,7 +15076,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15121,7 +15121,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15166,7 +15166,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15211,7 +15211,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15256,7 +15256,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15301,7 +15301,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15346,7 +15346,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15391,7 +15391,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15436,7 +15436,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15481,7 +15481,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15526,7 +15526,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15571,7 +15571,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15616,7 +15616,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15661,7 +15661,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15706,7 +15706,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15751,7 +15751,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15796,7 +15796,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15841,7 +15841,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15886,7 +15886,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15931,7 +15931,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16007,7 +16007,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Oktober!F40</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -16127,7 +16127,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -16637,7 +16637,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16682,7 +16682,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16727,7 +16727,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16772,7 +16772,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16817,7 +16817,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16862,7 +16862,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16907,7 +16907,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16952,7 +16952,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16997,7 +16997,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17042,7 +17042,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17087,7 +17087,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17132,7 +17132,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17177,7 +17177,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17222,7 +17222,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17267,7 +17267,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17312,7 +17312,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17357,7 +17357,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17402,7 +17402,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17447,7 +17447,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17492,7 +17492,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17537,7 +17537,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17582,7 +17582,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17627,7 +17627,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17672,7 +17672,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17717,7 +17717,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17762,7 +17762,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17807,7 +17807,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17852,7 +17852,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17897,7 +17897,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17942,7 +17942,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17987,7 +17987,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -18018,7 +18018,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">November!F40</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -18138,7 +18138,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -18728,7 +18728,7 @@
       </c>
       <c r="L4" s="133">
         <f>IF(April!K4&gt;0,April!K4,"")</f>
-        <v>0.19791666666666663</v>
+        <v>0.20833333333333337</v>
       </c>
       <c r="M4" s="120" t="str">
         <f>IF(OR(April!C4="",April!J4&lt;&gt;""),UPPER(April!J4),"F")</f>
@@ -19942,9 +19942,9 @@
         <f>April!A12</f>
         <v>44294</v>
       </c>
-      <c r="L12" s="134" t="str">
+      <c r="L12" s="134">
         <f>IF(April!K12&gt;0,April!K12,"")</f>
-        <v/>
+        <v>7.2916666666666741E-2</v>
       </c>
       <c r="M12" s="126" t="str">
         <f>IF(OR(April!C12="",April!J12&lt;&gt;""),UPPER(April!J12),"F")</f>
@@ -23499,7 +23499,7 @@
       <c r="J36" s="265"/>
       <c r="K36" s="413">
         <f>April!F38</f>
-        <v>0.19791666666666663</v>
+        <v>0.28125000000000011</v>
       </c>
       <c r="L36" s="413"/>
       <c r="M36" s="264"/>
@@ -23553,7 +23553,7 @@
       <c r="AK36" s="264"/>
       <c r="AL36" s="266">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.0833333333333335</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="1" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -23580,7 +23580,7 @@
       <c r="J37" s="83"/>
       <c r="K37" s="408">
         <f ca="1">ROUND(K36-K35,10)</f>
-        <v>0.19791666669999999</v>
+        <v>0.28125</v>
       </c>
       <c r="L37" s="408"/>
       <c r="M37" s="82"/>
@@ -23634,7 +23634,7 @@
       <c r="AK37" s="82"/>
       <c r="AL37" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.125</v>
+        <v>-2.0416666666999999</v>
       </c>
     </row>
     <row r="38" spans="1:38" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
@@ -23661,7 +23661,7 @@
       <c r="J38" s="410"/>
       <c r="K38" s="410">
         <f>April!J40</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L38" s="410"/>
       <c r="M38" s="410"/>
@@ -23715,7 +23715,7 @@
       <c r="AK38" s="410"/>
       <c r="AL38" s="343">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
@@ -26070,7 +26070,7 @@
       <c r="D2" s="92"/>
       <c r="E2" s="93">
         <f>Jahresübersicht!AL38</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -32828,7 +32828,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -32960,7 +32960,7 @@
         <v>0.4375</v>
       </c>
       <c r="E4" s="323">
-        <v>0.63541666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F4" s="323"/>
       <c r="G4" s="323"/>
@@ -32972,7 +32972,7 @@
       <c r="J4" s="299"/>
       <c r="K4" s="317">
         <f>IF(A4="",0,IF(IF(D4&lt;E4,E4-D4,IF(E4="",0,E4-D4+1))+IF(F4&lt;G4,G4-F4,IF(G4="",0,G4-F4+1))-H4&gt;0,IF(D4&lt;E4,E4-D4,IF(E4="",0,E4-D4+1))+IF(F4&lt;G4,G4-F4,IF(G4="",0,G4-F4+1))-H4,0))</f>
-        <v>0.19791666666666663</v>
+        <v>0.20833333333333337</v>
       </c>
       <c r="L4" s="318">
         <f t="shared" ref="L4:L34" ca="1" si="3">IF(AND(C4&lt;&gt;"",J4=""),IF(ISERROR(VLOOKUP(B4,Feiertage,2,FALSE)),0,VLOOKUP(B4,Feiertage,3,FALSE)*N4),IF(A4="",0,IF(J4&lt;&gt;"",IF(UPPER(J4)=VLOOKUP(UPPER(J4),Code,1,FALSE),IF(OR(VLOOKUP(J4,Code,2,FALSE)="NONE",VLOOKUP(J4,Code,2,FALSE)="XTRA",VLOOKUP(J4,Code,2,FALSE)="REST"),K4,IF(ISERROR(VLOOKUP(B4,Feiertage,2,FALSE)),VLOOKUP(J4,Code,2,FALSE)*N4,IF(VLOOKUP(B4,Feiertage,3,FALSE)=0.5,IF(OR(UPPER(J4)="G",UPPER(J4)="H"),VLOOKUP(B4,Feiertage,3,FALSE)*VLOOKUP(J4,Code,2,FALSE)*N4,0),VLOOKUP(B4,Feiertage,3,FALSE)*VLOOKUP(J4,Code,2,FALSE)*N4))),N4),N4)))</f>
@@ -32980,16 +32980,18 @@
       </c>
       <c r="M4" s="300">
         <f t="shared" ref="M4:M33" ca="1" si="4">IF(A4="",0,ROUND(K4-L4,14))</f>
-        <v>0.19791666666666999</v>
+        <v>0.20833333333333001</v>
       </c>
       <c r="N4" s="359">
         <f t="shared" ref="N4:N34" ca="1" si="5">IF(A4="",0,INDIRECT(ADDRESS(MATCH(A4,SOLL_AZ_Ab,1)+11,WEEKDAY(A4,2)+3,,,"Voreinstellungen"),TRUE))</f>
         <v>0</v>
       </c>
-      <c r="O4" s="301"/>
+      <c r="O4" s="301" t="s">
+        <v>144</v>
+      </c>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>1</v>
+        <v>1.0104166666666601</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33034,7 +33036,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>1</v>
+        <v>1.0104166666666601</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33079,7 +33081,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>1</v>
+        <v>1.0104166666666601</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33124,7 +33126,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0104166666666601</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33169,7 +33171,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0104166666666601</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33214,7 +33216,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0104166666666601</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33259,7 +33261,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0104166666666601</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33304,7 +33306,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0104166666666601</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33320,8 +33322,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D12" s="325"/>
-      <c r="E12" s="325"/>
+      <c r="D12" s="325">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E12" s="325">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="F12" s="325"/>
       <c r="G12" s="325"/>
       <c r="H12" s="326"/>
@@ -33332,7 +33338,7 @@
       <c r="J12" s="163"/>
       <c r="K12" s="319">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>7.2916666666666741E-2</v>
       </c>
       <c r="L12" s="320">
         <f t="shared" ca="1" si="3"/>
@@ -33340,16 +33346,18 @@
       </c>
       <c r="M12" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>7.2916666666670002E-2</v>
       </c>
       <c r="N12" s="360">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
-      <c r="O12" s="165"/>
+      <c r="O12" s="165" t="s">
+        <v>144</v>
+      </c>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33394,7 +33402,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33439,7 +33447,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33484,7 +33492,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33529,7 +33537,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33574,7 +33582,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33619,7 +33627,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33664,7 +33672,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33709,7 +33717,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33754,7 +33762,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33799,7 +33807,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33844,7 +33852,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33889,7 +33897,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33934,7 +33942,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -33979,7 +33987,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34024,7 +34032,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34069,7 +34077,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34114,7 +34122,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34159,7 +34167,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34204,7 +34212,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34249,7 +34257,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34294,7 +34302,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -34434,7 +34442,7 @@
       </c>
       <c r="F38" s="171">
         <f>SUM(K4:K34)</f>
-        <v>0.19791666666666663</v>
+        <v>0.28125000000000011</v>
       </c>
       <c r="G38" s="53"/>
       <c r="I38" s="68"/>
@@ -34490,13 +34498,13 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
       <c r="J40" s="210">
         <f>COUNTIF(K4:K34,"&gt;0")-IF(Voreinstellungen!C28="XTRA",COUNTIF(J4:J34,Voreinstellungen!B28),0)-IF(Voreinstellungen!C29="XTRA",COUNTIF(J4:J34,Voreinstellungen!B29),0)-IF(Voreinstellungen!C30="XTRA",COUNTIF(J4:J34,Voreinstellungen!B30),0)-IF(Voreinstellungen!C31="XTRA",COUNTIF(J4:J34,Voreinstellungen!B31),0)-IF(Voreinstellungen!C32="XTRA",COUNTIF(J4:J34,Voreinstellungen!B32),0)-IF(Voreinstellungen!C33="XTRA",COUNTIF(J4:J34,Voreinstellungen!B33),0)-COUNTIF(J4:J34,"H")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K40" s="380" t="s">
         <v>91</v>
@@ -35000,7 +35008,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35045,7 +35053,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35090,7 +35098,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35135,7 +35143,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35180,7 +35188,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35225,7 +35233,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35270,7 +35278,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35315,7 +35323,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35360,7 +35368,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35405,7 +35413,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35450,7 +35458,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35495,7 +35503,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35540,7 +35548,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35585,7 +35593,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35630,7 +35638,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35675,7 +35683,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35720,7 +35728,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35765,7 +35773,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35810,7 +35818,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35855,7 +35863,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35900,7 +35908,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35945,7 +35953,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -35990,7 +35998,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36035,7 +36043,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36080,7 +36088,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36125,7 +36133,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36170,7 +36178,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36215,7 +36223,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36260,7 +36268,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36305,7 +36313,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36350,7 +36358,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -36381,7 +36389,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">April!F40</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -36501,7 +36509,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -37011,7 +37019,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37056,7 +37064,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37101,7 +37109,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37146,7 +37154,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37191,7 +37199,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37236,7 +37244,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37281,7 +37289,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37326,7 +37334,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37371,7 +37379,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37416,7 +37424,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37461,7 +37469,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37506,7 +37514,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37551,7 +37559,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37596,7 +37604,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37641,7 +37649,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37686,7 +37694,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37731,7 +37739,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37776,7 +37784,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37821,7 +37829,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37866,7 +37874,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37911,7 +37919,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37956,7 +37964,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38001,7 +38009,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38046,7 +38054,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38091,7 +38099,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38136,7 +38144,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38181,7 +38189,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38226,7 +38234,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38271,7 +38279,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38316,7 +38324,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38392,7 +38400,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Mai!F40</f>
-        <v>1</v>
+        <v>1.0833333333333299</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -38512,7 +38520,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -39022,7 +39030,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39067,7 +39075,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39112,7 +39120,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39157,7 +39165,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39202,7 +39210,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39247,7 +39255,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39292,7 +39300,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39337,7 +39345,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39382,7 +39390,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39427,7 +39435,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39472,7 +39480,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39517,7 +39525,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39562,7 +39570,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39607,7 +39615,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39652,7 +39660,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39697,7 +39705,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39742,7 +39750,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39787,7 +39795,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39832,7 +39840,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39877,7 +39885,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39922,7 +39930,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39967,7 +39975,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40012,7 +40020,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40057,7 +40065,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40102,7 +40110,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40147,7 +40155,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40192,7 +40200,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40237,7 +40245,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40282,7 +40290,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40327,7 +40335,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40372,7 +40380,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -40403,7 +40411,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juni!F40</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -40523,7 +40531,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-2.125</v>
+        <v>-2.0416666666666701</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>

</xml_diff>

<commit_message>
Added UMAP and improved documentation
</commit_message>
<xml_diff>
--- a/Arbeitszeit.xlsx
+++ b/Arbeitszeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Philipp\Studium\Molecular-Test-Time-Adaptation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9690FED-B328-431A-8015-79B673D04AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04A4ECE-9188-4F03-9853-9F19D9CF0B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="HCoKw4gRij0gV6dkJfNeqDY8SK+w2PMaLYVl2wyqiuSEdbwXoxG0BpbDJ/qeWfNHoSNSKsH2JW6N7mRDHC8t+w==" workbookSaltValue="AxSev/HzJnlnx2x5wdOaWw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9420" tabRatio="933" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="145">
   <si>
     <t>Benutzer-Voreinstellungen</t>
   </si>
@@ -8593,7 +8593,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8638,7 +8638,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8683,7 +8683,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8728,7 +8728,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8773,7 +8773,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8818,7 +8818,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8863,7 +8863,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8908,7 +8908,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8953,7 +8953,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8998,7 +8998,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9043,7 +9043,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9088,7 +9088,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9133,7 +9133,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9178,7 +9178,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9223,7 +9223,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9268,7 +9268,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9313,7 +9313,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9358,7 +9358,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9403,7 +9403,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9448,7 +9448,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9493,7 +9493,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9538,7 +9538,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9583,7 +9583,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9628,7 +9628,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9673,7 +9673,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9718,7 +9718,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9763,7 +9763,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9808,7 +9808,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9853,7 +9853,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9898,7 +9898,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9943,7 +9943,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -9974,7 +9974,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juli!F40</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -10094,7 +10094,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -10604,7 +10604,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10649,7 +10649,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10694,7 +10694,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10739,7 +10739,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10784,7 +10784,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10829,7 +10829,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10874,7 +10874,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10919,7 +10919,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10964,7 +10964,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11009,7 +11009,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11054,7 +11054,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11099,7 +11099,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11144,7 +11144,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11189,7 +11189,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11234,7 +11234,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11279,7 +11279,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11324,7 +11324,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11369,7 +11369,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11414,7 +11414,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11459,7 +11459,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11504,7 +11504,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11549,7 +11549,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11594,7 +11594,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11639,7 +11639,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11684,7 +11684,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11729,7 +11729,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11774,7 +11774,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11819,7 +11819,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11864,7 +11864,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11909,7 +11909,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11985,7 +11985,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">August!F40</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -12105,7 +12105,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -12615,7 +12615,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12660,7 +12660,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12705,7 +12705,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12750,7 +12750,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12795,7 +12795,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12840,7 +12840,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12885,7 +12885,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12930,7 +12930,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12975,7 +12975,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13020,7 +13020,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13065,7 +13065,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13110,7 +13110,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13155,7 +13155,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13200,7 +13200,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13245,7 +13245,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13290,7 +13290,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13335,7 +13335,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13380,7 +13380,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13425,7 +13425,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13470,7 +13470,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13515,7 +13515,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13560,7 +13560,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13605,7 +13605,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13650,7 +13650,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13695,7 +13695,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13740,7 +13740,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13785,7 +13785,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13830,7 +13830,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13875,7 +13875,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13920,7 +13920,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13965,7 +13965,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -13996,7 +13996,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">September!F40</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -14116,7 +14116,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -14626,7 +14626,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14671,7 +14671,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14716,7 +14716,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14761,7 +14761,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14806,7 +14806,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14851,7 +14851,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14896,7 +14896,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14941,7 +14941,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14986,7 +14986,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15031,7 +15031,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15076,7 +15076,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15121,7 +15121,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15166,7 +15166,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15211,7 +15211,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15256,7 +15256,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15301,7 +15301,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15346,7 +15346,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15391,7 +15391,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15436,7 +15436,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15481,7 +15481,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15526,7 +15526,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15571,7 +15571,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15616,7 +15616,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15661,7 +15661,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15706,7 +15706,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15751,7 +15751,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15796,7 +15796,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15841,7 +15841,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15886,7 +15886,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15931,7 +15931,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16007,7 +16007,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Oktober!F40</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -16127,7 +16127,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -16637,7 +16637,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16682,7 +16682,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16727,7 +16727,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16772,7 +16772,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16817,7 +16817,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16862,7 +16862,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16907,7 +16907,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16952,7 +16952,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16997,7 +16997,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17042,7 +17042,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17087,7 +17087,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17132,7 +17132,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17177,7 +17177,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17222,7 +17222,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17267,7 +17267,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17312,7 +17312,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17357,7 +17357,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17402,7 +17402,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17447,7 +17447,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17492,7 +17492,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17537,7 +17537,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17582,7 +17582,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17627,7 +17627,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17672,7 +17672,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17717,7 +17717,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17762,7 +17762,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17807,7 +17807,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17852,7 +17852,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17897,7 +17897,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17942,7 +17942,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17987,7 +17987,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -18018,7 +18018,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">November!F40</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -18138,7 +18138,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -23146,9 +23146,9 @@
         <f>Mai!A33</f>
         <v>44345</v>
       </c>
-      <c r="O33" s="134" t="str">
+      <c r="O33" s="134">
         <f>IF(Mai!K33&gt;0,Mai!K33,"")</f>
-        <v/>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="P33" s="122" t="str">
         <f>IF(OR(Mai!C33="",Mai!J33&lt;&gt;""),UPPER(Mai!J33),"F")</f>
@@ -23505,7 +23505,7 @@
       <c r="M36" s="264"/>
       <c r="N36" s="421">
         <f>Mai!F38</f>
-        <v>0.20833333333333326</v>
+        <v>0.24999999999999989</v>
       </c>
       <c r="O36" s="421"/>
       <c r="P36" s="265"/>
@@ -23553,7 +23553,7 @@
       <c r="AK36" s="264"/>
       <c r="AL36" s="266">
         <f t="shared" si="0"/>
-        <v>1.9895833333333333</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="1" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -23586,7 +23586,7 @@
       <c r="M37" s="82"/>
       <c r="N37" s="418">
         <f ca="1">ROUND(N36-N35,10)</f>
-        <v>0.20833333330000001</v>
+        <v>0.25</v>
       </c>
       <c r="O37" s="418"/>
       <c r="P37" s="83"/>
@@ -23634,7 +23634,7 @@
       <c r="AK37" s="82"/>
       <c r="AL37" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1354166667000001</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="38" spans="1:38" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
@@ -23667,7 +23667,7 @@
       <c r="M38" s="424"/>
       <c r="N38" s="424">
         <f>Mai!J40</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O38" s="424"/>
       <c r="P38" s="424"/>
@@ -23715,7 +23715,7 @@
       <c r="AK38" s="424"/>
       <c r="AL38" s="343">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
@@ -26070,7 +26070,7 @@
       <c r="D2" s="92"/>
       <c r="E2" s="93">
         <f>Jahresübersicht!AL38</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -34881,7 +34881,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -36326,8 +36326,12 @@
         <f>IF(ISERROR(VLOOKUP(A33,Feiertage,2,FALSE)),"",(VLOOKUP(A33,Feiertage,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="D33" s="325"/>
-      <c r="E33" s="325"/>
+      <c r="D33" s="325">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="E33" s="325">
+        <v>0.84375</v>
+      </c>
       <c r="F33" s="325"/>
       <c r="G33" s="325"/>
       <c r="H33" s="326"/>
@@ -36338,7 +36342,7 @@
       <c r="J33" s="163"/>
       <c r="K33" s="319">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="L33" s="320">
         <f t="shared" ca="1" si="3"/>
@@ -36346,16 +36350,18 @@
       </c>
       <c r="M33" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>4.1666666666670002E-2</v>
       </c>
       <c r="N33" s="360">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
-      <c r="O33" s="165"/>
+      <c r="O33" s="165" t="s">
+        <v>144</v>
+      </c>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333399</v>
+        <v>2.0312500000000102</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -36400,7 +36406,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>1.9895833333333399</v>
+        <v>2.0312500000000102</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -36495,7 +36501,7 @@
       </c>
       <c r="F38" s="171">
         <f>SUM(K4:K34)</f>
-        <v>0.20833333333333326</v>
+        <v>0.24999999999999989</v>
       </c>
       <c r="G38" s="53"/>
       <c r="I38" s="68"/>
@@ -36551,13 +36557,13 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
       <c r="J40" s="210">
         <f>COUNTIF(K4:K34,"&gt;0")-IF(Voreinstellungen!C28="XTRA",COUNTIF(J4:J34,Voreinstellungen!B28),0)-IF(Voreinstellungen!C29="XTRA",COUNTIF(J4:J34,Voreinstellungen!B29),0)-IF(Voreinstellungen!C30="XTRA",COUNTIF(J4:J34,Voreinstellungen!B30),0)-IF(Voreinstellungen!C31="XTRA",COUNTIF(J4:J34,Voreinstellungen!B31),0)-IF(Voreinstellungen!C32="XTRA",COUNTIF(J4:J34,Voreinstellungen!B32),0)-IF(Voreinstellungen!C33="XTRA",COUNTIF(J4:J34,Voreinstellungen!B33),0)-COUNTIF(J4:J34,"H")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K40" s="380" t="s">
         <v>91</v>
@@ -37061,7 +37067,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37106,7 +37112,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37151,7 +37157,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37196,7 +37202,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37241,7 +37247,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37286,7 +37292,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37331,7 +37337,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37376,7 +37382,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37421,7 +37427,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37466,7 +37472,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37511,7 +37517,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37556,7 +37562,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37601,7 +37607,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37646,7 +37652,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37691,7 +37697,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37736,7 +37742,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37781,7 +37787,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37826,7 +37832,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37871,7 +37877,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37916,7 +37922,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37961,7 +37967,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38006,7 +38012,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38051,7 +38057,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38096,7 +38102,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38141,7 +38147,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38186,7 +38192,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38231,7 +38237,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38276,7 +38282,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38321,7 +38327,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38366,7 +38372,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38442,7 +38448,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Mai!F40</f>
-        <v>1.9895833333333299</v>
+        <v>2.03125</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -38562,7 +38568,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -39072,7 +39078,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39117,7 +39123,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39162,7 +39168,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39207,7 +39213,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39252,7 +39258,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39297,7 +39303,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39342,7 +39348,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39387,7 +39393,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39432,7 +39438,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39477,7 +39483,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39522,7 +39528,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39567,7 +39573,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39612,7 +39618,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39657,7 +39663,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39702,7 +39708,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39747,7 +39753,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39792,7 +39798,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39837,7 +39843,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39882,7 +39888,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39927,7 +39933,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39972,7 +39978,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40017,7 +40023,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40062,7 +40068,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40107,7 +40113,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40152,7 +40158,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40197,7 +40203,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40242,7 +40248,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40287,7 +40293,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40332,7 +40338,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40377,7 +40383,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40422,7 +40428,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -40453,7 +40459,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juni!F40</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -40573,7 +40579,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-1.1354166666666701</v>
+        <v>-1.09375</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>

</xml_diff>

<commit_message>
Added residual, layernorm, n_steps
</commit_message>
<xml_diff>
--- a/Arbeitszeit.xlsx
+++ b/Arbeitszeit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Philipp\Studium\Molecular-Test-Time-Adaptation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1602F80F-2EA6-41CA-A64B-7E2DBC150EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23158837-6262-4876-86C9-43EFE78DE2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="HCoKw4gRij0gV6dkJfNeqDY8SK+w2PMaLYVl2wyqiuSEdbwXoxG0BpbDJ/qeWfNHoSNSKsH2JW6N7mRDHC8t+w==" workbookSaltValue="AxSev/HzJnlnx2x5wdOaWw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-27840" yWindow="-3750" windowWidth="21600" windowHeight="11775" tabRatio="933" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="146">
   <si>
     <t>Benutzer-Voreinstellungen</t>
   </si>
@@ -8596,7 +8596,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8641,7 +8641,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8686,7 +8686,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8731,7 +8731,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8776,7 +8776,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8821,7 +8821,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8866,7 +8866,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8911,7 +8911,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8956,7 +8956,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9001,7 +9001,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9046,7 +9046,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9091,7 +9091,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9136,7 +9136,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9181,7 +9181,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9226,7 +9226,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9271,7 +9271,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9316,7 +9316,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9361,7 +9361,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9406,7 +9406,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9451,7 +9451,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9496,7 +9496,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9541,7 +9541,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9586,7 +9586,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9631,7 +9631,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9676,7 +9676,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9721,7 +9721,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9766,7 +9766,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9811,7 +9811,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9856,7 +9856,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9901,7 +9901,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9946,7 +9946,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -9977,7 +9977,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juli!F40</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -10097,7 +10097,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -10607,7 +10607,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10652,7 +10652,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10697,7 +10697,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10742,7 +10742,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10787,7 +10787,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10832,7 +10832,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10877,7 +10877,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10922,7 +10922,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10967,7 +10967,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11012,7 +11012,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11057,7 +11057,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11102,7 +11102,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11147,7 +11147,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11192,7 +11192,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11237,7 +11237,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11282,7 +11282,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11327,7 +11327,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11372,7 +11372,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11417,7 +11417,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11462,7 +11462,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11507,7 +11507,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11552,7 +11552,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11597,7 +11597,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11642,7 +11642,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11687,7 +11687,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11732,7 +11732,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11777,7 +11777,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11822,7 +11822,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11867,7 +11867,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11912,7 +11912,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11988,7 +11988,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">August!F40</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -12108,7 +12108,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -12618,7 +12618,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12663,7 +12663,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12708,7 +12708,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12753,7 +12753,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12798,7 +12798,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12843,7 +12843,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12888,7 +12888,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12933,7 +12933,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12978,7 +12978,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13023,7 +13023,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13068,7 +13068,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13113,7 +13113,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13158,7 +13158,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13203,7 +13203,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13248,7 +13248,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13293,7 +13293,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13338,7 +13338,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13383,7 +13383,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13428,7 +13428,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13473,7 +13473,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13518,7 +13518,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13563,7 +13563,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13608,7 +13608,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13653,7 +13653,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13698,7 +13698,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13743,7 +13743,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13788,7 +13788,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13833,7 +13833,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13878,7 +13878,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13923,7 +13923,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13968,7 +13968,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -13999,7 +13999,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">September!F40</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -14119,7 +14119,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -14629,7 +14629,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14674,7 +14674,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14719,7 +14719,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14764,7 +14764,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14809,7 +14809,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14854,7 +14854,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14899,7 +14899,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14944,7 +14944,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14989,7 +14989,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15034,7 +15034,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15079,7 +15079,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15124,7 +15124,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15169,7 +15169,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15214,7 +15214,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15259,7 +15259,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15304,7 +15304,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15349,7 +15349,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15394,7 +15394,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15439,7 +15439,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15484,7 +15484,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15529,7 +15529,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15574,7 +15574,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15619,7 +15619,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15664,7 +15664,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15709,7 +15709,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15754,7 +15754,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15799,7 +15799,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15844,7 +15844,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15889,7 +15889,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15934,7 +15934,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16010,7 +16010,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Oktober!F40</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -16130,7 +16130,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -16640,7 +16640,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16685,7 +16685,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16730,7 +16730,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16775,7 +16775,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16820,7 +16820,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16865,7 +16865,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16910,7 +16910,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16955,7 +16955,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17000,7 +17000,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17045,7 +17045,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17090,7 +17090,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17135,7 +17135,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17180,7 +17180,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17225,7 +17225,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17270,7 +17270,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17315,7 +17315,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17360,7 +17360,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17405,7 +17405,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17450,7 +17450,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17495,7 +17495,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17540,7 +17540,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17585,7 +17585,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17630,7 +17630,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17675,7 +17675,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17720,7 +17720,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17765,7 +17765,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17810,7 +17810,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17855,7 +17855,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17900,7 +17900,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17945,7 +17945,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17990,7 +17990,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -18021,7 +18021,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">November!F40</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -18141,7 +18141,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -19209,9 +19209,9 @@
         <f>Juni!A7</f>
         <v>44350</v>
       </c>
-      <c r="R7" s="134" t="str">
+      <c r="R7" s="134">
         <f>IF(Juni!K7&gt;0,Juni!K7,"")</f>
-        <v/>
+        <v>0.27083333333333326</v>
       </c>
       <c r="S7" s="126" t="str">
         <f>IF(OR(Juni!C7="",Juni!J7&lt;&gt;""),UPPER(Juni!J7),"F")</f>
@@ -23514,7 +23514,7 @@
       <c r="P36" s="265"/>
       <c r="Q36" s="420">
         <f>Juni!F38</f>
-        <v>0.76041666666666663</v>
+        <v>1.03125</v>
       </c>
       <c r="R36" s="420"/>
       <c r="S36" s="264"/>
@@ -23556,7 +23556,7 @@
       <c r="AK36" s="264"/>
       <c r="AL36" s="266">
         <f t="shared" si="0"/>
-        <v>2.8124999999999996</v>
+        <v>3.083333333333333</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="1" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -23595,7 +23595,7 @@
       <c r="P37" s="83"/>
       <c r="Q37" s="423">
         <f ca="1">ROUND(Q36-Q35,10)</f>
-        <v>-2.3645833333000001</v>
+        <v>-2.09375</v>
       </c>
       <c r="R37" s="423"/>
       <c r="S37" s="82"/>
@@ -23637,7 +23637,7 @@
       <c r="AK37" s="82"/>
       <c r="AL37" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.3125</v>
+        <v>-4.1666666699999855E-2</v>
       </c>
     </row>
     <row r="38" spans="1:38" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
@@ -23676,7 +23676,7 @@
       <c r="P38" s="424"/>
       <c r="Q38" s="424">
         <f>Juni!J40</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R38" s="424"/>
       <c r="S38" s="424"/>
@@ -23718,7 +23718,7 @@
       <c r="AK38" s="424"/>
       <c r="AL38" s="343">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
@@ -26073,7 +26073,7 @@
       <c r="D2" s="92"/>
       <c r="E2" s="93">
         <f>Jahresübersicht!AL38</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -36919,7 +36919,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -37200,8 +37200,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D7" s="325"/>
-      <c r="E7" s="325"/>
+      <c r="D7" s="325">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E7" s="325">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="F7" s="325"/>
       <c r="G7" s="325"/>
       <c r="H7" s="326"/>
@@ -37212,7 +37216,7 @@
       <c r="J7" s="163"/>
       <c r="K7" s="319">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.27083333333333326</v>
       </c>
       <c r="L7" s="320">
         <f t="shared" ca="1" si="3"/>
@@ -37220,16 +37224,18 @@
       </c>
       <c r="M7" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>0.27083333333332998</v>
       </c>
       <c r="N7" s="360">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
-      <c r="O7" s="165"/>
+      <c r="O7" s="165" t="s">
+        <v>144</v>
+      </c>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37274,7 +37280,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37319,7 +37325,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37364,7 +37370,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37409,7 +37415,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37454,7 +37460,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37499,7 +37505,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37544,7 +37550,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37589,7 +37595,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37634,7 +37640,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37679,7 +37685,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37724,7 +37730,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37769,7 +37775,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37814,7 +37820,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37859,7 +37865,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37904,7 +37910,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37949,7 +37955,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37994,7 +38000,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38039,7 +38045,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38084,7 +38090,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38129,7 +38135,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38174,7 +38180,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38219,7 +38225,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38264,7 +38270,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38309,7 +38315,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38354,7 +38360,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8125</v>
+        <v>3.0833333333333299</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38399,7 +38405,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38539,7 +38545,7 @@
       </c>
       <c r="F38" s="171">
         <f>SUM(K4:K34)</f>
-        <v>0.76041666666666663</v>
+        <v>1.03125</v>
       </c>
       <c r="G38" s="53"/>
       <c r="I38" s="68"/>
@@ -38595,13 +38601,13 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
       <c r="J40" s="210">
         <f>COUNTIF(K4:K34,"&gt;0")-IF(Voreinstellungen!C28="XTRA",COUNTIF(J4:J34,Voreinstellungen!B28),0)-IF(Voreinstellungen!C29="XTRA",COUNTIF(J4:J34,Voreinstellungen!B29),0)-IF(Voreinstellungen!C30="XTRA",COUNTIF(J4:J34,Voreinstellungen!B30),0)-IF(Voreinstellungen!C31="XTRA",COUNTIF(J4:J34,Voreinstellungen!B31),0)-IF(Voreinstellungen!C32="XTRA",COUNTIF(J4:J34,Voreinstellungen!B32),0)-IF(Voreinstellungen!C33="XTRA",COUNTIF(J4:J34,Voreinstellungen!B33),0)-COUNTIF(J4:J34,"H")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K40" s="380" t="s">
         <v>91</v>
@@ -39105,7 +39111,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39150,7 +39156,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39195,7 +39201,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39240,7 +39246,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39285,7 +39291,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39330,7 +39336,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39375,7 +39381,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39420,7 +39426,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39465,7 +39471,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39510,7 +39516,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39555,7 +39561,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39600,7 +39606,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39645,7 +39651,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39690,7 +39696,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39735,7 +39741,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39780,7 +39786,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39825,7 +39831,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39870,7 +39876,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39915,7 +39921,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39960,7 +39966,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40005,7 +40011,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40050,7 +40056,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40095,7 +40101,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40140,7 +40146,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40185,7 +40191,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40230,7 +40236,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40275,7 +40281,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40320,7 +40326,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40365,7 +40371,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40410,7 +40416,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40455,7 +40461,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -40486,7 +40492,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juni!F40</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -40606,7 +40612,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-0.3125</v>
+        <v>-4.1666666666670002E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>

</xml_diff>

<commit_message>
More Decoder Regularization, Hyperparam Opt
</commit_message>
<xml_diff>
--- a/Arbeitszeit.xlsx
+++ b/Arbeitszeit.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Philipp\Studium\Molecular-Test-Time-Adaptation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23158837-6262-4876-86C9-43EFE78DE2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D2AD99-0FEF-4D20-9C33-6A97050760FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="HCoKw4gRij0gV6dkJfNeqDY8SK+w2PMaLYVl2wyqiuSEdbwXoxG0BpbDJ/qeWfNHoSNSKsH2JW6N7mRDHC8t+w==" workbookSaltValue="AxSev/HzJnlnx2x5wdOaWw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-27840" yWindow="-3750" windowWidth="21600" windowHeight="11775" tabRatio="933" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" tabRatio="933" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Voreinstellungen" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="146">
   <si>
     <t>Benutzer-Voreinstellungen</t>
   </si>
@@ -8596,7 +8596,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8641,7 +8641,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8686,7 +8686,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8731,7 +8731,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8776,7 +8776,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8821,7 +8821,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8866,7 +8866,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8911,7 +8911,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -8956,7 +8956,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9001,7 +9001,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9046,7 +9046,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9091,7 +9091,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9136,7 +9136,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9181,7 +9181,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9226,7 +9226,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9271,7 +9271,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9316,7 +9316,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9361,7 +9361,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9406,7 +9406,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9451,7 +9451,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9496,7 +9496,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9541,7 +9541,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9586,7 +9586,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9631,7 +9631,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9676,7 +9676,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9721,7 +9721,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9766,7 +9766,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9811,7 +9811,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9856,7 +9856,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9901,7 +9901,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -9946,7 +9946,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -9977,7 +9977,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juli!F40</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -10097,7 +10097,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -10607,7 +10607,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10652,7 +10652,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10697,7 +10697,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10742,7 +10742,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10787,7 +10787,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10832,7 +10832,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10877,7 +10877,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10922,7 +10922,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -10967,7 +10967,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11012,7 +11012,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11057,7 +11057,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11102,7 +11102,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11147,7 +11147,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11192,7 +11192,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11237,7 +11237,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11282,7 +11282,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11327,7 +11327,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11372,7 +11372,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11417,7 +11417,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11462,7 +11462,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11507,7 +11507,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11552,7 +11552,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11597,7 +11597,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11642,7 +11642,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11687,7 +11687,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11732,7 +11732,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11777,7 +11777,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11822,7 +11822,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11867,7 +11867,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11912,7 +11912,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11988,7 +11988,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">August!F40</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -12108,7 +12108,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -12618,7 +12618,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12663,7 +12663,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12708,7 +12708,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12753,7 +12753,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12798,7 +12798,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12843,7 +12843,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12888,7 +12888,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12933,7 +12933,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -12978,7 +12978,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13023,7 +13023,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13068,7 +13068,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13113,7 +13113,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13158,7 +13158,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13203,7 +13203,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13248,7 +13248,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13293,7 +13293,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13338,7 +13338,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13383,7 +13383,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13428,7 +13428,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13473,7 +13473,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13518,7 +13518,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13563,7 +13563,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13608,7 +13608,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13653,7 +13653,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13698,7 +13698,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13743,7 +13743,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13788,7 +13788,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13833,7 +13833,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13878,7 +13878,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13923,7 +13923,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -13968,7 +13968,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -13999,7 +13999,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">September!F40</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -14119,7 +14119,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -14629,7 +14629,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14674,7 +14674,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14719,7 +14719,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14764,7 +14764,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14809,7 +14809,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14854,7 +14854,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14899,7 +14899,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14944,7 +14944,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -14989,7 +14989,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15034,7 +15034,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15079,7 +15079,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15124,7 +15124,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15169,7 +15169,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15214,7 +15214,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15259,7 +15259,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15304,7 +15304,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15349,7 +15349,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15394,7 +15394,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15439,7 +15439,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15484,7 +15484,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15529,7 +15529,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15574,7 +15574,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15619,7 +15619,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15664,7 +15664,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15709,7 +15709,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15754,7 +15754,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15799,7 +15799,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15844,7 +15844,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15889,7 +15889,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -15934,7 +15934,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16010,7 +16010,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Oktober!F40</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -16130,7 +16130,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -16640,7 +16640,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16685,7 +16685,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16730,7 +16730,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16775,7 +16775,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16820,7 +16820,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16865,7 +16865,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16910,7 +16910,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -16955,7 +16955,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17000,7 +17000,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17045,7 +17045,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17090,7 +17090,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17135,7 +17135,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17180,7 +17180,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17225,7 +17225,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17270,7 +17270,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17315,7 +17315,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17360,7 +17360,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17405,7 +17405,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17450,7 +17450,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17495,7 +17495,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17540,7 +17540,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17585,7 +17585,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17630,7 +17630,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17675,7 +17675,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17720,7 +17720,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17765,7 +17765,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17810,7 +17810,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17855,7 +17855,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17900,7 +17900,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17945,7 +17945,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -17990,7 +17990,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -18021,7 +18021,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">November!F40</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -18141,7 +18141,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
@@ -19361,9 +19361,9 @@
         <f>Juni!A8</f>
         <v>44351</v>
       </c>
-      <c r="R8" s="134" t="str">
+      <c r="R8" s="134">
         <f>IF(Juni!K8&gt;0,Juni!K8,"")</f>
-        <v/>
+        <v>0.10416666666666674</v>
       </c>
       <c r="S8" s="126" t="str">
         <f>IF(OR(Juni!C8="",Juni!J8&lt;&gt;""),UPPER(Juni!J8),"F")</f>
@@ -23514,7 +23514,7 @@
       <c r="P36" s="265"/>
       <c r="Q36" s="420">
         <f>Juni!F38</f>
-        <v>1.03125</v>
+        <v>1.1354166666666667</v>
       </c>
       <c r="R36" s="420"/>
       <c r="S36" s="264"/>
@@ -23556,7 +23556,7 @@
       <c r="AK36" s="264"/>
       <c r="AL36" s="266">
         <f t="shared" si="0"/>
-        <v>3.083333333333333</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="37" spans="1:38" s="1" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
@@ -23595,7 +23595,7 @@
       <c r="P37" s="83"/>
       <c r="Q37" s="423">
         <f ca="1">ROUND(Q36-Q35,10)</f>
-        <v>-2.09375</v>
+        <v>-1.9895833332999999</v>
       </c>
       <c r="R37" s="423"/>
       <c r="S37" s="82"/>
@@ -23637,7 +23637,7 @@
       <c r="AK37" s="82"/>
       <c r="AL37" s="84">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.1666666699999855E-2</v>
+        <v>6.2500000000000222E-2</v>
       </c>
     </row>
     <row r="38" spans="1:38" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
@@ -23676,7 +23676,7 @@
       <c r="P38" s="424"/>
       <c r="Q38" s="424">
         <f>Juni!J40</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R38" s="424"/>
       <c r="S38" s="424"/>
@@ -23718,7 +23718,7 @@
       <c r="AK38" s="424"/>
       <c r="AL38" s="343">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
@@ -26073,7 +26073,7 @@
       <c r="D2" s="92"/>
       <c r="E2" s="93">
         <f>Jahresübersicht!AL38</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -36919,7 +36919,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -37251,8 +37251,12 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D8" s="325"/>
-      <c r="E8" s="325"/>
+      <c r="D8" s="325">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E8" s="325">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="F8" s="325"/>
       <c r="G8" s="325"/>
       <c r="H8" s="326"/>
@@ -37263,7 +37267,7 @@
       <c r="J8" s="163"/>
       <c r="K8" s="319">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.10416666666666674</v>
       </c>
       <c r="L8" s="320">
         <f t="shared" ca="1" si="3"/>
@@ -37271,16 +37275,18 @@
       </c>
       <c r="M8" s="164">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>0.10416666666667</v>
       </c>
       <c r="N8" s="360">
         <f t="shared" ca="1" si="5"/>
         <v>0</v>
       </c>
-      <c r="O8" s="165"/>
+      <c r="O8" s="165" t="s">
+        <v>144</v>
+      </c>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37325,7 +37331,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37370,7 +37376,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37415,7 +37421,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37460,7 +37466,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37505,7 +37511,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37550,7 +37556,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37595,7 +37601,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37640,7 +37646,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37685,7 +37691,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37730,7 +37736,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37775,7 +37781,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37820,7 +37826,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37865,7 +37871,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37910,7 +37916,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -37955,7 +37961,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38000,7 +38006,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38045,7 +38051,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38090,7 +38096,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38135,7 +38141,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38180,7 +38186,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38225,7 +38231,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38270,7 +38276,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38315,7 +38321,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38360,7 +38366,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>3.0833333333333299</v>
+        <v>3.1875</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38405,7 +38411,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -38545,7 +38551,7 @@
       </c>
       <c r="F38" s="171">
         <f>SUM(K4:K34)</f>
-        <v>1.03125</v>
+        <v>1.1354166666666667</v>
       </c>
       <c r="G38" s="53"/>
       <c r="I38" s="68"/>
@@ -38601,13 +38607,13 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>
       <c r="J40" s="210">
         <f>COUNTIF(K4:K34,"&gt;0")-IF(Voreinstellungen!C28="XTRA",COUNTIF(J4:J34,Voreinstellungen!B28),0)-IF(Voreinstellungen!C29="XTRA",COUNTIF(J4:J34,Voreinstellungen!B29),0)-IF(Voreinstellungen!C30="XTRA",COUNTIF(J4:J34,Voreinstellungen!B30),0)-IF(Voreinstellungen!C31="XTRA",COUNTIF(J4:J34,Voreinstellungen!B31),0)-IF(Voreinstellungen!C32="XTRA",COUNTIF(J4:J34,Voreinstellungen!B32),0)-IF(Voreinstellungen!C33="XTRA",COUNTIF(J4:J34,Voreinstellungen!B33),0)-COUNTIF(J4:J34,"H")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K40" s="380" t="s">
         <v>91</v>
@@ -39111,7 +39117,7 @@
       <c r="O4" s="301"/>
       <c r="P4" s="302">
         <f ca="1">IF(A4="","",IF(M4&lt;&gt;"",ROUND(F36+M4,14),F36))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39156,7 +39162,7 @@
       <c r="O5" s="165"/>
       <c r="P5" s="304">
         <f ca="1">IF(A5="","",IF(M5&lt;&gt;"",ROUND(P4+M5,14),P4))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39201,7 +39207,7 @@
       <c r="O6" s="165"/>
       <c r="P6" s="304">
         <f t="shared" ref="P6:P33" ca="1" si="8">IF(A6="","",IF(M6&lt;&gt;"",ROUND(P5+M6,14),P5))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39246,7 +39252,7 @@
       <c r="O7" s="165"/>
       <c r="P7" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39291,7 +39297,7 @@
       <c r="O8" s="165"/>
       <c r="P8" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39336,7 +39342,7 @@
       <c r="O9" s="165"/>
       <c r="P9" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39381,7 +39387,7 @@
       <c r="O10" s="165"/>
       <c r="P10" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39426,7 +39432,7 @@
       <c r="O11" s="165"/>
       <c r="P11" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39471,7 +39477,7 @@
       <c r="O12" s="165"/>
       <c r="P12" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39516,7 +39522,7 @@
       <c r="O13" s="165"/>
       <c r="P13" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39561,7 +39567,7 @@
       <c r="O14" s="165"/>
       <c r="P14" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39606,7 +39612,7 @@
       <c r="O15" s="165"/>
       <c r="P15" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39651,7 +39657,7 @@
       <c r="O16" s="165"/>
       <c r="P16" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="17" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39696,7 +39702,7 @@
       <c r="O17" s="165"/>
       <c r="P17" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="18" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39741,7 +39747,7 @@
       <c r="O18" s="165"/>
       <c r="P18" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39786,7 +39792,7 @@
       <c r="O19" s="165"/>
       <c r="P19" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="20" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39831,7 +39837,7 @@
       <c r="O20" s="165"/>
       <c r="P20" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39876,7 +39882,7 @@
       <c r="O21" s="165"/>
       <c r="P21" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39921,7 +39927,7 @@
       <c r="O22" s="165"/>
       <c r="P22" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -39966,7 +39972,7 @@
       <c r="O23" s="165"/>
       <c r="P23" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40011,7 +40017,7 @@
       <c r="O24" s="165"/>
       <c r="P24" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="25" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40056,7 +40062,7 @@
       <c r="O25" s="165"/>
       <c r="P25" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="26" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40101,7 +40107,7 @@
       <c r="O26" s="165"/>
       <c r="P26" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="27" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40146,7 +40152,7 @@
       <c r="O27" s="165"/>
       <c r="P27" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40191,7 +40197,7 @@
       <c r="O28" s="165"/>
       <c r="P28" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40236,7 +40242,7 @@
       <c r="O29" s="165"/>
       <c r="P29" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40281,7 +40287,7 @@
       <c r="O30" s="165"/>
       <c r="P30" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="31" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40326,7 +40332,7 @@
       <c r="O31" s="165"/>
       <c r="P31" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40371,7 +40377,7 @@
       <c r="O32" s="165"/>
       <c r="P32" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40416,7 +40422,7 @@
       <c r="O33" s="165"/>
       <c r="P33" s="304">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="24" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -40461,7 +40467,7 @@
       <c r="O34" s="310"/>
       <c r="P34" s="311">
         <f ca="1">IF(A34="","",IF(M34&lt;&gt;"",ROUND(P33+M34,14),P33))</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="35" spans="1:16" s="24" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -40492,7 +40498,7 @@
       </c>
       <c r="F36" s="169">
         <f ca="1">Juni!F40</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G36" s="53"/>
       <c r="I36" s="68"/>
@@ -40612,7 +40618,7 @@
       </c>
       <c r="F40" s="172">
         <f ca="1">ROUND(F38+F36-F39-F37,14)</f>
-        <v>-4.1666666666670002E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="G40" s="53"/>
       <c r="I40" s="70"/>

</xml_diff>